<commit_message>
Code avec la colonne Avance quinzaine
</commit_message>
<xml_diff>
--- a/Output/LOVAHARITIANA Hoby_S-100.xlsx
+++ b/Output/LOVAHARITIANA Hoby_S-100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CE PC\Desktop\FicheDePaie\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E30CB5E-89A7-4694-A04A-5245FC820F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DC14D57-3D96-4FB9-AF41-DD4FBF77EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="990" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1380" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2176,7 +2176,6 @@
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="46">
-        <f>+[1]SUD!AD15</f>
         <v>0</v>
       </c>
       <c r="E50" s="22"/>

</xml_diff>

<commit_message>
Version finale Fiche de Paie ANKA Madagascar
</commit_message>
<xml_diff>
--- a/Output/LOVAHARITIANA Hoby_S-100.xlsx
+++ b/Output/LOVAHARITIANA Hoby_S-100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CE PC\Desktop\FicheDePaie\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DC14D57-3D96-4FB9-AF41-DD4FBF77EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B620C414-6DB0-4251-99DF-C52B1A96842D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1380" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="2550" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>

</xml_diff>